<commit_message>
update agendas to pull attachments
</commit_message>
<xml_diff>
--- a/inputs/GR Excel Agenda.xlsx
+++ b/inputs/GR Excel Agenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jspenc35\projects\curriculog_excel_sheet_generator\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD11D303-7115-4D21-9450-5496B8C8F3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214B9E97-B838-4765-B8EF-E5B84A419F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="177">
   <si>
     <t>Field</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>2025-2026 GR Add Course; 2025-2026 GR Revise Course; 2025-2026 GR Revise Program; 2025-2026 GR Add Program; 2025-2026 GR Change Course Number / Subject / Department; 2025-2026 GR Change Program Name / Department; 2025-2026 GR Drop Course; 2025-2026 GR End Program; Other Form; New Prefix/Subject Code (Graduate); Update Approval Tree(s) / Update Originator(s); Agenda Form - Administrative Use Only (Impact Sorting); New Degree Code; Informational Items; EL Designated Courses Reassessment; Courses Not Taught in 4 Years; Committee Reports; Content and Text Change (Non-Program Requirements); Correction Items</t>
+  </si>
+  <si>
+    <t>attachments</t>
   </si>
 </sst>
 </file>
@@ -1054,27 +1057,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809DB27-F851-4238-909D-DC6D276C789A}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="228.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="228.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -1142,13 +1145,13 @@
         <v>18</v>
       </c>
       <c r="C4" s="8">
-        <v>45673</v>
+        <v>45722</v>
       </c>
       <c r="E4" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1159,28 +1162,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1194,25 +1202,25 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B$4:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B72:B296</xm:sqref>
+          <xm:sqref>B73:B297</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this to include an additional field from the proposal as a comment in the cell. Good for fields in the proposal that has lots of text.  " xr:uid="{B019C073-487B-47B8-8ABF-602FE6834B7C}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>F12:F23 F2:F5 F7:F9</xm:sqref>
+          <xm:sqref>F13:F24 F2:F5 F7:F10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field to separate sheets by. Creates a separate sheet for each unique value in the field. If the field is &quot;College&quot; and the proposals are from A&amp;S and Tickle Engineering, a sheet titled A&amp;S and a sheet titled Tickle Engineering are created." xr:uid="{CCE53851-1D4A-4889-8217-59A49DFAA977}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>J11 J7:J9 J2:J4</xm:sqref>
+          <xm:sqref>J12 J7:J10 J2:J4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select the field from the proposal you want in your Excel spreadsheet._x000a_" xr:uid="{ED19FA7F-0466-4F44-81DE-819E52E3AFC1}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A5 A7:A77</xm:sqref>
+          <xm:sqref>A2:A5 A7:A78</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
           <x14:formula1>
@@ -1224,13 +1232,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B5 B7:B71</xm:sqref>
+          <xm:sqref>B2:B5 B7:B72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A32929B-C51D-4A5A-BFA3-4B20B2A647A4}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H5 H7:H26</xm:sqref>
+          <xm:sqref>H2:H5 H7:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1240,24 +1248,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A8F092-27DE-412E-8E0F-037E456B2861}">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView topLeftCell="A132" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="94.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1268,7 +1276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1290,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1306,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1306,7 +1314,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1322,7 +1330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1330,7 +1338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1338,724 +1346,729 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>